<commit_message>
fixed tables and codebooks
</commit_message>
<xml_diff>
--- a/Projects/blubbi90/StandardOperatingProcedureLayout/Datasets/codebooks/1. Overview.xlsx
+++ b/Projects/blubbi90/StandardOperatingProcedureLayout/Datasets/codebooks/1. Overview.xlsx
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Ablauf</t>
   </si>
   <si>
-    <t xml:space="preserve">[Image Overview]</t>
+    <t xml:space="preserve">[Image_overview]</t>
   </si>
 </sst>
 </file>
@@ -169,7 +169,7 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Open Sans"/>
       <family val="2"/>
       <charset val="1"/>
@@ -177,7 +177,7 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Open Sans"/>
       <family val="2"/>
       <charset val="1"/>
@@ -232,7 +232,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,19 +245,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -453,7 +461,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -464,7 +472,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -478,120 +486,120 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4"/>
+      <c r="B10" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>